<commit_message>
Fixed bug in DCOPF to consider storage
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/3 node battery opf.xlsx
+++ b/Grids_and_profiles/grids/3 node battery opf.xlsx
@@ -99,10 +99,10 @@
     <t>0j</t>
   </si>
   <si>
-    <t>-773.0</t>
-  </si>
-  <si>
-    <t>-466.0</t>
+    <t>-1191.0</t>
+  </si>
+  <si>
+    <t>-716.0</t>
   </si>
   <si>
     <t>60.0</t>
@@ -111,19 +111,19 @@
     <t>Bus 2</t>
   </si>
   <si>
-    <t>-1039.0</t>
-  </si>
-  <si>
-    <t>-611.0</t>
+    <t>-1457.0</t>
+  </si>
+  <si>
+    <t>-861.0</t>
   </si>
   <si>
     <t>Bus 3</t>
   </si>
   <si>
-    <t>-901.0</t>
-  </si>
-  <si>
-    <t>-324.0</t>
+    <t>-1319.0</t>
+  </si>
+  <si>
+    <t>-574.0</t>
   </si>
   <si>
     <t>bus_from</t>
@@ -210,7 +210,7 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>batt</t>
+    <t>batt1@Bus 3</t>
   </si>
   <si>
     <t>Y</t>
@@ -880,7 +880,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="n">
-        <v>9.999999999999999e-21</v>
+        <v>0.05</v>
       </c>
       <c r="K2" t="n">
         <v>9.999999999999999e-21</v>
@@ -927,7 +927,7 @@
         <v>0.02</v>
       </c>
       <c r="J3" t="n">
-        <v>9.999999999999999e-21</v>
+        <v>0.08</v>
       </c>
       <c r="K3" t="n">
         <v>9.999999999999999e-21</v>
@@ -971,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>9.999999999999999e-21</v>
+        <v>0.01</v>
       </c>
       <c r="J4" t="n">
-        <v>9.999999999999999e-21</v>
+        <v>0.06</v>
       </c>
       <c r="K4" t="n">
         <v>9.999999999999999e-21</v>

</xml_diff>